<commit_message>
Update document - ACER
</commit_message>
<xml_diff>
--- a/Working/Test annexture.xlsx
+++ b/Working/Test annexture.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asiri\Documents\GitHub\Undergraduate-Final-Year-Project-\Working\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Documents\GitHub\Undergraduate-Final-Year-Project-\Working\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAD0DF0C-99FE-4E77-B829-AC8E12C1F663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91AA84B9-292F-46BC-B525-45D4AB9614B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test cases" sheetId="1" r:id="rId1"/>
+    <sheet name="Test Evaluation" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>Scenario</t>
   </si>
@@ -91,13 +92,40 @@
   </si>
   <si>
     <t>Lassana sindhu tikak gaga inne nethuwa puke amarauwata illang kagattha moda moosalaya</t>
+  </si>
+  <si>
+    <t>Naïve Bayes</t>
+  </si>
+  <si>
+    <t>Logistic Regression</t>
+  </si>
+  <si>
+    <t>Decision Tree</t>
+  </si>
+  <si>
+    <t>Random Forest</t>
+  </si>
+  <si>
+    <t>SVM</t>
+  </si>
+  <si>
+    <t>Deep Learnig</t>
+  </si>
+  <si>
+    <t>transformers</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Percentage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,8 +133,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -119,8 +155,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -143,16 +185,109 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,46 +570,46 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="95.109375" customWidth="1"/>
+    <col min="2" max="2" width="95.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="2" t="s">
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -485,7 +620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -499,7 +634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -510,7 +645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -524,7 +659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -538,7 +673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -552,7 +687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -563,7 +698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -580,7 +715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -591,7 +726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -602,7 +737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -616,7 +751,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -627,7 +762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -644,7 +779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -658,7 +793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -672,52 +807,112 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18">
+    <row r="18" spans="1:6" ht="29.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:6" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="29.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="20" spans="1:6" ht="29.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="1:6" ht="29.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="1:6" ht="29.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="1:6" ht="29.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="1:6" ht="29.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="25" spans="1:6" ht="29.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="26" spans="1:6" ht="29.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="1:6" ht="29.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="1:6" ht="29.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="1:6" ht="29.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="1:6" ht="29.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="1:6" ht="29.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="1:6" ht="29.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="33" ht="29.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="34" ht="29.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="35" ht="29.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="36" ht="29.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="37" ht="29.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="38" ht="29.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="39" ht="29.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="40" ht="29.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="41" ht="29.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="42" ht="29.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="43" ht="29.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="44" ht="29.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="45" ht="29.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="46" ht="29.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="47" ht="29.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="48" ht="29.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="49" ht="29.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="50" ht="29.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="51" ht="29.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="52" ht="29.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="53" ht="29.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="54" ht="29.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="55" ht="29.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="56" ht="29.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="57" ht="29.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="58" ht="29.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="59" ht="29.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:6" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" ht="29.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="1:1" ht="29.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="1:1" ht="29.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="1:1" ht="29.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="1:1" ht="29.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:1" ht="29.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:1" ht="29.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:1" ht="29.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:1" ht="29.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:1" ht="29.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:1" ht="29.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:1" ht="29.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:1" ht="29.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:1" ht="29.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" ht="29.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="29.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="29.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" ht="29.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" ht="29.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" ht="29.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" ht="29.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" ht="29.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" ht="29.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" ht="29.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" ht="29.45" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="D1:F1"/>
@@ -727,4 +922,232 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25544B06-7C5F-4146-BD02-89400E65E816}">
+  <dimension ref="A1:R8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="5">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6">
+        <v>4</v>
+      </c>
+      <c r="F1" s="6">
+        <v>5</v>
+      </c>
+      <c r="G1" s="6">
+        <v>6</v>
+      </c>
+      <c r="H1" s="6">
+        <v>7</v>
+      </c>
+      <c r="I1" s="6">
+        <v>8</v>
+      </c>
+      <c r="J1" s="6">
+        <v>9</v>
+      </c>
+      <c r="K1" s="6">
+        <v>10</v>
+      </c>
+      <c r="L1" s="6">
+        <v>11</v>
+      </c>
+      <c r="M1" s="6">
+        <v>12</v>
+      </c>
+      <c r="N1" s="6">
+        <v>13</v>
+      </c>
+      <c r="O1" s="6">
+        <v>14</v>
+      </c>
+      <c r="P1" s="7">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="R1" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+    </row>
+    <row r="3" spans="1:18" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+    </row>
+    <row r="4" spans="1:18" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+    </row>
+    <row r="5" spans="1:18" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+    </row>
+    <row r="6" spans="1:18" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+    </row>
+    <row r="7" spans="1:18" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+    </row>
+    <row r="8" spans="1:18" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
UPDATE DOC AND CODE - ACER
</commit_message>
<xml_diff>
--- a/Working/Test annexture.xlsx
+++ b/Working/Test annexture.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Documents\GitHub\Undergraduate-Final-Year-Project-\Working\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91AA84B9-292F-46BC-B525-45D4AB9614B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{491EED7B-BA1C-4D79-B9F6-B4075BE8970B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test cases" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="38">
   <si>
     <t>Scenario</t>
   </si>
@@ -70,9 +70,6 @@
     <t>Oba thuma thamai me rata balaporoththu una wenasa. Oba thuma matha thamai hamoma wishwasaya thibbe. Malimawata jaya!</t>
   </si>
   <si>
-    <t xml:space="preserve"> pamko biththare size eke madine kekara gapu tharamata?? Nodakin danwath paurashaya thiyagena vihuluwak novi paduwe idapan humthoo</t>
-  </si>
-  <si>
     <t>anna ehema thithata wad karoth nam katawath pissu kelinnawath boruwen minissu rawattannawath bari wei</t>
   </si>
   <si>
@@ -119,6 +116,30 @@
   </si>
   <si>
     <t>Percentage</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>TP</t>
+  </si>
+  <si>
+    <t>FP</t>
+  </si>
+  <si>
+    <t>FN</t>
+  </si>
+  <si>
+    <t>TN</t>
+  </si>
+  <si>
+    <t>pamko biththare size eke madine kekara gapu tharamata?? Nodakin danwath paurashaya thiyagena vihuluwak novi paduwe idapan humthoo</t>
   </si>
 </sst>
 </file>
@@ -142,7 +163,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -158,6 +179,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -263,12 +290,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -282,12 +306,25 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -570,8 +607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,25 +617,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
       <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
@@ -703,7 +740,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -720,7 +757,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -731,7 +768,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -742,7 +779,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -756,7 +793,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -767,7 +804,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -784,7 +821,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -798,7 +835,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -926,226 +963,1105 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25544B06-7C5F-4146-BD02-89400E65E816}">
-  <dimension ref="A1:R8"/>
+  <dimension ref="A1:V21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W16" sqref="W16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.28515625" customWidth="1"/>
+    <col min="2" max="16" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="5">
-        <v>1</v>
-      </c>
-      <c r="C1" s="6">
+    <row r="1" spans="1:22" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="4">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5">
         <v>2</v>
       </c>
-      <c r="D1" s="6">
+      <c r="D1" s="5">
         <v>3</v>
       </c>
-      <c r="E1" s="6">
+      <c r="E1" s="5">
         <v>4</v>
       </c>
-      <c r="F1" s="6">
+      <c r="F1" s="5">
         <v>5</v>
       </c>
-      <c r="G1" s="6">
+      <c r="G1" s="5">
         <v>6</v>
       </c>
-      <c r="H1" s="6">
+      <c r="H1" s="5">
         <v>7</v>
       </c>
-      <c r="I1" s="6">
+      <c r="I1" s="5">
         <v>8</v>
       </c>
-      <c r="J1" s="6">
+      <c r="J1" s="5">
         <v>9</v>
       </c>
-      <c r="K1" s="6">
+      <c r="K1" s="5">
         <v>10</v>
       </c>
-      <c r="L1" s="6">
+      <c r="L1" s="5">
         <v>11</v>
       </c>
-      <c r="M1" s="6">
+      <c r="M1" s="5">
         <v>12</v>
       </c>
-      <c r="N1" s="6">
+      <c r="N1" s="5">
         <v>13</v>
       </c>
-      <c r="O1" s="6">
+      <c r="O1" s="5">
         <v>14</v>
       </c>
-      <c r="P1" s="7">
+      <c r="P1" s="6">
         <v>15</v>
       </c>
-      <c r="Q1" s="11" t="s">
+      <c r="Q1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="R1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="R1" s="11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="S1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="V1" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4">
+        <v>0</v>
+      </c>
+      <c r="C2" s="5">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5">
+        <v>0</v>
+      </c>
+      <c r="E2" s="5">
+        <v>1</v>
+      </c>
+      <c r="F2" s="5">
+        <v>1</v>
+      </c>
+      <c r="G2" s="5">
+        <v>1</v>
+      </c>
+      <c r="H2" s="5">
+        <v>0</v>
+      </c>
+      <c r="I2" s="5">
+        <v>1</v>
+      </c>
+      <c r="J2" s="5">
+        <v>0</v>
+      </c>
+      <c r="K2" s="5">
+        <v>0</v>
+      </c>
+      <c r="L2" s="5">
+        <v>1</v>
+      </c>
+      <c r="M2" s="5">
+        <v>0</v>
+      </c>
+      <c r="N2" s="5">
+        <v>1</v>
+      </c>
+      <c r="O2" s="5">
+        <v>1</v>
+      </c>
+      <c r="P2" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+    </row>
+    <row r="3" spans="1:22" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="O3" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="P3" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>10</v>
+      </c>
+      <c r="R3" s="2">
+        <v>66.67</v>
+      </c>
+      <c r="S3">
+        <v>6</v>
+      </c>
+      <c r="T3">
+        <v>4</v>
+      </c>
+      <c r="U3">
+        <v>2</v>
+      </c>
+      <c r="V3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="11"/>
+      <c r="B4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="O4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="P4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>8</v>
+      </c>
+      <c r="R4" s="2">
+        <v>53.33</v>
+      </c>
+      <c r="S4">
+        <v>5</v>
+      </c>
+      <c r="T4">
+        <v>3</v>
+      </c>
+      <c r="U4">
+        <v>3</v>
+      </c>
+      <c r="V4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-    </row>
-    <row r="3" spans="1:18" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="B5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="N5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="O5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="P5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>11</v>
+      </c>
+      <c r="R5" s="2">
+        <v>73.33</v>
+      </c>
+      <c r="S5">
+        <v>7</v>
+      </c>
+      <c r="T5">
+        <v>4</v>
+      </c>
+      <c r="U5">
+        <v>2</v>
+      </c>
+      <c r="V5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="11"/>
+      <c r="B6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="N6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="O6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="P6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>9</v>
+      </c>
+      <c r="R6" s="2">
+        <v>60</v>
+      </c>
+      <c r="S6">
+        <v>3</v>
+      </c>
+      <c r="T6">
+        <v>6</v>
+      </c>
+      <c r="U6">
+        <v>3</v>
+      </c>
+      <c r="V6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="3"/>
-    </row>
-    <row r="4" spans="1:18" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="B7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="N7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="O7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="P7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>11</v>
+      </c>
+      <c r="R7" s="2">
+        <v>73.33</v>
+      </c>
+      <c r="S7">
+        <v>8</v>
+      </c>
+      <c r="T7">
+        <v>3</v>
+      </c>
+      <c r="U7">
+        <v>3</v>
+      </c>
+      <c r="V7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="11"/>
+      <c r="B8" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="M8" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="N8" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="O8" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="P8" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>9</v>
+      </c>
+      <c r="R8" s="2">
+        <v>60</v>
+      </c>
+      <c r="S8">
+        <v>8</v>
+      </c>
+      <c r="T8">
+        <v>1</v>
+      </c>
+      <c r="U8">
+        <v>5</v>
+      </c>
+      <c r="V8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
-      <c r="R4" s="3"/>
-    </row>
-    <row r="5" spans="1:18" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="B9" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="L9" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="M9" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="N9" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="O9" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="P9" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>12</v>
+      </c>
+      <c r="R9" s="2">
+        <v>80</v>
+      </c>
+      <c r="S9">
+        <v>8</v>
+      </c>
+      <c r="T9">
+        <v>4</v>
+      </c>
+      <c r="U9">
+        <v>2</v>
+      </c>
+      <c r="V9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="11"/>
+      <c r="B10" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="L10" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="M10" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="N10" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="O10" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="P10" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>11</v>
+      </c>
+      <c r="R10" s="2">
+        <v>73.33</v>
+      </c>
+      <c r="S10">
+        <v>9</v>
+      </c>
+      <c r="T10">
+        <v>2</v>
+      </c>
+      <c r="U10">
+        <v>4</v>
+      </c>
+      <c r="V10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="3"/>
-      <c r="R5" s="3"/>
-    </row>
-    <row r="6" spans="1:18" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="B11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="L11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="M11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="N11" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="O11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="P11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>10</v>
+      </c>
+      <c r="R11" s="2">
+        <v>66.67</v>
+      </c>
+      <c r="S11">
+        <v>6</v>
+      </c>
+      <c r="T11">
+        <v>4</v>
+      </c>
+      <c r="U11">
+        <v>2</v>
+      </c>
+      <c r="V11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="11"/>
+      <c r="B12" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="L12" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="M12" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="N12" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="O12" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="P12" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q12" s="2">
+        <v>8</v>
+      </c>
+      <c r="R12" s="2">
+        <v>53.33</v>
+      </c>
+      <c r="S12">
+        <v>5</v>
+      </c>
+      <c r="T12">
+        <v>3</v>
+      </c>
+      <c r="U12">
+        <v>3</v>
+      </c>
+      <c r="V12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="3"/>
-      <c r="R6" s="3"/>
-    </row>
-    <row r="7" spans="1:18" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="B13" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="L13" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="M13" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="N13" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="O13" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="P13" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q13" s="13">
+        <v>9</v>
+      </c>
+      <c r="R13" s="2">
+        <v>60</v>
+      </c>
+      <c r="S13">
+        <v>9</v>
+      </c>
+      <c r="T13">
+        <v>0</v>
+      </c>
+      <c r="U13">
+        <v>6</v>
+      </c>
+      <c r="V13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="11"/>
+      <c r="B14" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="K14" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="L14" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="M14" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="N14" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="O14" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="P14" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q14" s="13">
+        <v>9</v>
+      </c>
+      <c r="R14" s="2">
+        <v>60</v>
+      </c>
+      <c r="S14">
+        <v>9</v>
+      </c>
+      <c r="T14">
+        <v>0</v>
+      </c>
+      <c r="U14">
+        <v>6</v>
+      </c>
+      <c r="V14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="3"/>
-      <c r="R7" s="3"/>
-    </row>
-    <row r="8" spans="1:18" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="3"/>
-      <c r="R8" s="3"/>
+      <c r="B15" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="K15" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="L15" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="M15" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="N15" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="O15" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="P15" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q15" s="13">
+        <v>7</v>
+      </c>
+      <c r="R15" s="2">
+        <v>46.66</v>
+      </c>
+      <c r="S15">
+        <v>2</v>
+      </c>
+      <c r="T15">
+        <v>5</v>
+      </c>
+      <c r="U15">
+        <v>1</v>
+      </c>
+      <c r="V15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="11"/>
+      <c r="B16" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="K16" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="L16" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="M16" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="N16" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="O16" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="P16" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q16" s="13">
+        <v>10</v>
+      </c>
+      <c r="R16" s="2">
+        <v>66.67</v>
+      </c>
+      <c r="S16">
+        <v>9</v>
+      </c>
+      <c r="T16">
+        <v>1</v>
+      </c>
+      <c r="U16">
+        <v>5</v>
+      </c>
+      <c r="V16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update project - ACER
</commit_message>
<xml_diff>
--- a/Working/Test annexture.xlsx
+++ b/Working/Test annexture.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Documents\GitHub\Undergraduate-Final-Year-Project-\Working\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{491EED7B-BA1C-4D79-B9F6-B4075BE8970B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6CCF104-D3AA-4EF5-84B3-387282E7C941}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test cases" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="45">
   <si>
     <t>Scenario</t>
   </si>
@@ -140,6 +140,27 @@
   </si>
   <si>
     <t>pamko biththare size eke madine kekara gapu tharamata?? Nodakin danwath paurashaya thiyagena vihuluwak novi paduwe idapan humthoo</t>
+  </si>
+  <si>
+    <t>TPR</t>
+  </si>
+  <si>
+    <t>FPR</t>
+  </si>
+  <si>
+    <t>TNR</t>
+  </si>
+  <si>
+    <t>Actual</t>
+  </si>
+  <si>
+    <t>TEST EVALUATION TABLE</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>Precision</t>
   </si>
 </sst>
 </file>
@@ -163,7 +184,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -179,12 +200,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -290,7 +305,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -309,9 +324,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -321,10 +333,30 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -607,8 +639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -617,25 +649,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="8" t="s">
+      <c r="A1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
       <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
@@ -963,10 +995,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25544B06-7C5F-4146-BD02-89400E65E816}">
-  <dimension ref="A1:V21"/>
+  <dimension ref="A1:AA22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W16" sqref="W16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AA14" sqref="AA14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -975,462 +1007,460 @@
     <col min="2" max="16" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="4">
-        <v>1</v>
-      </c>
-      <c r="C1" s="5">
+    <row r="1" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+    </row>
+    <row r="2" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5">
         <v>2</v>
       </c>
-      <c r="D1" s="5">
+      <c r="D2" s="5">
         <v>3</v>
       </c>
-      <c r="E1" s="5">
+      <c r="E2" s="5">
         <v>4</v>
       </c>
-      <c r="F1" s="5">
+      <c r="F2" s="5">
         <v>5</v>
       </c>
-      <c r="G1" s="5">
+      <c r="G2" s="5">
         <v>6</v>
       </c>
-      <c r="H1" s="5">
+      <c r="H2" s="5">
         <v>7</v>
       </c>
-      <c r="I1" s="5">
+      <c r="I2" s="5">
         <v>8</v>
       </c>
-      <c r="J1" s="5">
+      <c r="J2" s="5">
         <v>9</v>
       </c>
-      <c r="K1" s="5">
+      <c r="K2" s="5">
         <v>10</v>
       </c>
-      <c r="L1" s="5">
+      <c r="L2" s="5">
         <v>11</v>
       </c>
-      <c r="M1" s="5">
+      <c r="M2" s="5">
         <v>12</v>
       </c>
-      <c r="N1" s="5">
+      <c r="N2" s="5">
         <v>13</v>
       </c>
-      <c r="O1" s="5">
+      <c r="O2" s="5">
         <v>14</v>
       </c>
-      <c r="P1" s="6">
+      <c r="P2" s="6">
         <v>15</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="Q2" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="R2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="S2" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="T2" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="U1" s="7" t="s">
+      <c r="U2" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="V1" s="7" t="s">
+      <c r="V2" s="7" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" spans="1:22" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="4">
+      <c r="W2" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="X2" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z2" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA2" s="20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="4">
         <v>0</v>
       </c>
-      <c r="C2" s="5">
-        <v>1</v>
-      </c>
-      <c r="D2" s="5">
+      <c r="C3" s="5">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5">
         <v>0</v>
       </c>
-      <c r="E2" s="5">
-        <v>1</v>
-      </c>
-      <c r="F2" s="5">
-        <v>1</v>
-      </c>
-      <c r="G2" s="5">
-        <v>1</v>
-      </c>
-      <c r="H2" s="5">
+      <c r="E3" s="5">
+        <v>1</v>
+      </c>
+      <c r="F3" s="5">
+        <v>1</v>
+      </c>
+      <c r="G3" s="5">
+        <v>1</v>
+      </c>
+      <c r="H3" s="5">
         <v>0</v>
       </c>
-      <c r="I2" s="5">
-        <v>1</v>
-      </c>
-      <c r="J2" s="5">
+      <c r="I3" s="5">
+        <v>1</v>
+      </c>
+      <c r="J3" s="5">
         <v>0</v>
       </c>
-      <c r="K2" s="5">
+      <c r="K3" s="5">
         <v>0</v>
       </c>
-      <c r="L2" s="5">
-        <v>1</v>
-      </c>
-      <c r="M2" s="5">
+      <c r="L3" s="5">
+        <v>1</v>
+      </c>
+      <c r="M3" s="5">
         <v>0</v>
       </c>
-      <c r="N2" s="5">
-        <v>1</v>
-      </c>
-      <c r="O2" s="5">
-        <v>1</v>
-      </c>
-      <c r="P2" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
-    </row>
-    <row r="3" spans="1:22" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="N3" s="5">
+        <v>1</v>
+      </c>
+      <c r="O3" s="5">
+        <v>1</v>
+      </c>
+      <c r="P3" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="7"/>
+    </row>
+    <row r="4" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="M3" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="N3" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="O3" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="P3" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q3" s="1">
+      <c r="B4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="O4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="P4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q4" s="16">
         <v>10</v>
       </c>
-      <c r="R3" s="2">
+      <c r="R4" s="2">
         <v>66.67</v>
       </c>
-      <c r="S3">
+      <c r="S4">
         <v>6</v>
       </c>
-      <c r="T3">
+      <c r="T4">
         <v>4</v>
-      </c>
-      <c r="U3">
-        <v>2</v>
-      </c>
-      <c r="V3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="L4" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="M4" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="N4" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="O4" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="P4" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q4" s="2">
-        <v>8</v>
-      </c>
-      <c r="R4" s="2">
-        <v>53.33</v>
-      </c>
-      <c r="S4">
-        <v>5</v>
-      </c>
-      <c r="T4">
-        <v>3</v>
       </c>
       <c r="U4">
         <v>3</v>
       </c>
       <c r="V4">
+        <v>2</v>
+      </c>
+      <c r="W4">
+        <v>0.75</v>
+      </c>
+      <c r="X4">
+        <v>0.42</v>
+      </c>
+      <c r="Y4">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="AA4">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10"/>
+      <c r="B5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="N5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="O5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="P5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q5" s="16">
+        <v>8</v>
+      </c>
+      <c r="R5" s="2">
+        <v>53.33</v>
+      </c>
+      <c r="S5">
+        <v>5</v>
+      </c>
+      <c r="T5">
+        <v>3</v>
+      </c>
+      <c r="U5">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:22" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="V5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="L5" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="M5" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="N5" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="O5" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="P5" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q5" s="1">
+      <c r="B6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="N6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="O6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="P6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q6" s="16">
         <v>11</v>
       </c>
-      <c r="R5" s="2">
+      <c r="R6" s="2">
         <v>73.33</v>
       </c>
-      <c r="S5">
+      <c r="S6">
         <v>7</v>
       </c>
-      <c r="T5">
+      <c r="T6">
         <v>4</v>
       </c>
-      <c r="U5">
+      <c r="U6">
         <v>2</v>
       </c>
-      <c r="V5">
+      <c r="V6">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:22" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
-      <c r="B6" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="L6" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="M6" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="N6" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="O6" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="P6" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q6" s="2">
+      <c r="W6" s="13">
+        <v>0.77</v>
+      </c>
+      <c r="X6" s="14">
+        <v>0.33</v>
+      </c>
+      <c r="Y6" s="14">
+        <v>0.66</v>
+      </c>
+      <c r="Z6" s="14"/>
+      <c r="AA6" s="14">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="10"/>
+      <c r="B7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="N7" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="O7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="P7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q7" s="16">
         <v>9</v>
       </c>
-      <c r="R6" s="2">
+      <c r="R7" s="2">
         <v>60</v>
       </c>
-      <c r="S6">
+      <c r="S7">
         <v>3</v>
       </c>
-      <c r="T6">
+      <c r="T7">
         <v>6</v>
-      </c>
-      <c r="U6">
-        <v>3</v>
-      </c>
-      <c r="V6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="K7" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="L7" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="M7" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="N7" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="O7" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="P7" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q7" s="1">
-        <v>11</v>
-      </c>
-      <c r="R7" s="2">
-        <v>73.33</v>
-      </c>
-      <c r="S7">
-        <v>8</v>
-      </c>
-      <c r="T7">
-        <v>3</v>
       </c>
       <c r="U7">
         <v>3</v>
       </c>
       <c r="V7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="B8" s="7" t="s">
         <v>30</v>
       </c>
@@ -1438,7 +1468,7 @@
         <v>30</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>30</v>
@@ -1459,7 +1489,7 @@
         <v>31</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L8" s="7" t="s">
         <v>31</v>
@@ -1476,29 +1506,40 @@
       <c r="P8" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="Q8" s="2">
-        <v>9</v>
+      <c r="Q8" s="16">
+        <v>11</v>
       </c>
       <c r="R8" s="2">
-        <v>60</v>
+        <v>73.33</v>
       </c>
       <c r="S8">
         <v>8</v>
       </c>
       <c r="T8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="U8">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="V8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
-        <v>24</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="W8" s="13">
+        <v>0.72</v>
+      </c>
+      <c r="X8" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="Y8" s="14">
+        <v>0.75</v>
+      </c>
+      <c r="Z8" s="14"/>
+      <c r="AA8" s="14">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="10"/>
       <c r="B9" s="7" t="s">
         <v>30</v>
       </c>
@@ -1506,7 +1547,7 @@
         <v>30</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>30</v>
@@ -1518,7 +1559,7 @@
         <v>30</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I9" s="7" t="s">
         <v>30</v>
@@ -1527,7 +1568,7 @@
         <v>31</v>
       </c>
       <c r="K9" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L9" s="7" t="s">
         <v>31</v>
@@ -1544,295 +1585,322 @@
       <c r="P9" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="Q9" s="1">
-        <v>12</v>
+      <c r="Q9" s="16">
+        <v>9</v>
       </c>
       <c r="R9" s="2">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="S9">
         <v>8</v>
       </c>
       <c r="T9">
+        <v>1</v>
+      </c>
+      <c r="U9">
+        <v>1</v>
+      </c>
+      <c r="V9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="L10" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="M10" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="N10" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="O10" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="P10" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q10" s="16">
+        <v>12</v>
+      </c>
+      <c r="R10" s="2">
+        <v>80</v>
+      </c>
+      <c r="S10">
+        <v>8</v>
+      </c>
+      <c r="T10">
         <v>4</v>
       </c>
-      <c r="U9">
+      <c r="U10">
+        <v>1</v>
+      </c>
+      <c r="V10">
         <v>2</v>
       </c>
-      <c r="V9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
-      <c r="B10" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="J10" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="K10" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="L10" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="M10" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="N10" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="O10" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="P10" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q10" s="2">
+      <c r="W10" s="13">
+        <v>0.8</v>
+      </c>
+      <c r="X10" s="14">
+        <v>0.2</v>
+      </c>
+      <c r="Y10" s="14">
+        <v>0.8</v>
+      </c>
+      <c r="Z10" s="14"/>
+      <c r="AA10" s="14">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10"/>
+      <c r="B11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="L11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="M11" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="N11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="O11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="P11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q11" s="16">
         <v>11</v>
       </c>
-      <c r="R10" s="2">
+      <c r="R11" s="2">
         <v>73.33</v>
       </c>
-      <c r="S10">
+      <c r="S11">
         <v>9</v>
       </c>
-      <c r="T10">
+      <c r="T11">
         <v>2</v>
       </c>
-      <c r="U10">
+      <c r="U11">
+        <v>0</v>
+      </c>
+      <c r="V11">
         <v>4</v>
       </c>
-      <c r="V10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+    </row>
+    <row r="12" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="J11" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="K11" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="L11" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="M11" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="N11" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="O11" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="P11" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q11" s="1">
+      <c r="B12" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="L12" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="M12" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="N12" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="O12" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="P12" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q12" s="16">
         <v>10</v>
       </c>
-      <c r="R11" s="2">
+      <c r="R12" s="2">
         <v>66.67</v>
       </c>
-      <c r="S11">
+      <c r="S12">
         <v>6</v>
       </c>
-      <c r="T11">
+      <c r="T12">
         <v>4</v>
-      </c>
-      <c r="U11">
-        <v>2</v>
-      </c>
-      <c r="V11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
-      <c r="B12" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="I12" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="J12" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="K12" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="L12" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="M12" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="N12" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="O12" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="P12" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q12" s="2">
-        <v>8</v>
-      </c>
-      <c r="R12" s="2">
-        <v>53.33</v>
-      </c>
-      <c r="S12">
-        <v>5</v>
-      </c>
-      <c r="T12">
-        <v>3</v>
       </c>
       <c r="U12">
         <v>3</v>
       </c>
       <c r="V12">
+        <v>2</v>
+      </c>
+      <c r="W12">
+        <v>0.75</v>
+      </c>
+      <c r="X12">
+        <v>0.42</v>
+      </c>
+      <c r="Y12">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="AA12">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10"/>
+      <c r="B13" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="L13" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="M13" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="N13" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="O13" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="P13" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q13" s="16">
+        <v>8</v>
+      </c>
+      <c r="R13" s="2">
+        <v>53.33</v>
+      </c>
+      <c r="S13">
+        <v>5</v>
+      </c>
+      <c r="T13">
+        <v>3</v>
+      </c>
+      <c r="U13">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:22" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+      <c r="V13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="J13" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="K13" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="L13" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="M13" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="N13" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="O13" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="P13" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q13" s="13">
-        <v>9</v>
-      </c>
-      <c r="R13" s="2">
-        <v>60</v>
-      </c>
-      <c r="S13">
-        <v>9</v>
-      </c>
-      <c r="T13">
-        <v>0</v>
-      </c>
-      <c r="U13">
-        <v>6</v>
-      </c>
-      <c r="V13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
       <c r="B14" s="7" t="s">
         <v>31</v>
       </c>
@@ -1878,7 +1946,7 @@
       <c r="P14" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="Q14" s="13">
+      <c r="Q14" s="16">
         <v>9</v>
       </c>
       <c r="R14" s="2">
@@ -1891,102 +1959,102 @@
         <v>0</v>
       </c>
       <c r="U14">
+        <v>0</v>
+      </c>
+      <c r="V14">
         <v>6</v>
       </c>
-      <c r="V14">
+    </row>
+    <row r="15" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="10"/>
+      <c r="B15" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="K15" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="L15" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="M15" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="N15" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="O15" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="P15" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q15" s="16">
+        <v>9</v>
+      </c>
+      <c r="R15" s="2">
+        <v>60</v>
+      </c>
+      <c r="S15">
+        <v>9</v>
+      </c>
+      <c r="T15">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:22" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="12" t="s">
+      <c r="U15">
+        <v>0</v>
+      </c>
+      <c r="V15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B16" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" s="7" t="s">
+      <c r="C16" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="H15" s="7" t="s">
+      <c r="E16" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H16" s="7" t="s">
         <v>32</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="J15" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="K15" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="L15" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="M15" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="N15" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="O15" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="P15" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q15" s="13">
-        <v>7</v>
-      </c>
-      <c r="R15" s="2">
-        <v>46.66</v>
-      </c>
-      <c r="S15">
-        <v>2</v>
-      </c>
-      <c r="T15">
-        <v>5</v>
-      </c>
-      <c r="U15">
-        <v>1</v>
-      </c>
-      <c r="V15">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
-      <c r="B16" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>31</v>
       </c>
       <c r="I16" s="7" t="s">
         <v>32</v>
@@ -1995,75 +2063,144 @@
         <v>31</v>
       </c>
       <c r="K16" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="L16" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="M16" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="M16" s="7" t="s">
-        <v>30</v>
-      </c>
       <c r="N16" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O16" s="7" t="s">
         <v>32</v>
       </c>
       <c r="P16" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q16" s="16">
+        <v>7</v>
+      </c>
+      <c r="R16" s="2">
+        <v>46.66</v>
+      </c>
+      <c r="S16">
+        <v>2</v>
+      </c>
+      <c r="T16">
+        <v>5</v>
+      </c>
+      <c r="U16">
+        <v>7</v>
+      </c>
+      <c r="V16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="10"/>
+      <c r="B17" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="Q16" s="13">
+      <c r="D17" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="K17" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="L17" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="M17" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="N17" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="O17" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="P17" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q17" s="16">
         <v>10</v>
       </c>
-      <c r="R16" s="2">
+      <c r="R17" s="2">
         <v>66.67</v>
       </c>
-      <c r="S16">
+      <c r="S17">
         <v>9</v>
       </c>
-      <c r="T16">
-        <v>1</v>
-      </c>
-      <c r="U16">
+      <c r="T17">
+        <v>1</v>
+      </c>
+      <c r="U17">
+        <v>0</v>
+      </c>
+      <c r="V17">
         <v>5</v>
       </c>
-      <c r="V16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    </row>
+    <row r="19" spans="1:22" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>33</v>
       </c>
-      <c r="B18">
+      <c r="B19">
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="20" spans="1:22" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>34</v>
       </c>
-      <c r="B19">
+      <c r="B20">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="21" spans="1:22" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>35</v>
       </c>
-      <c r="B20">
+      <c r="B21">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="22" spans="1:22" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>36</v>
       </c>
-      <c r="B21">
+      <c r="B22">
         <v>4</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:R1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>